<commit_message>
Test Trigger selftest added; Test Trigger bug fixes and code maintenance
</commit_message>
<xml_diff>
--- a/test/documentation/ReturnValueHandling.xlsx
+++ b/test/documentation/ReturnValueHandling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RobotTest\projects\ROBFW_AIO\RobotFramework_AIO\test\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D654D47E-FF2C-42A3-8108-AA831D3C2F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F86BAC-6630-4E95-A042-9E8AE061C71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="230" windowWidth="18580" windowHeight="9920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="435" windowWidth="24855" windowHeight="15765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terms" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Application</t>
   </si>
@@ -101,11 +101,28 @@
     <t>no internal error / no error of any Executor</t>
   </si>
   <si>
+    <t>-x (with x is the number of  Executors who returned a value != 0)</t>
+  </si>
+  <si>
+    <t>Test Trigger
+self test</t>
+  </si>
+  <si>
+    <t>no internal error / error of any Test Trigger</t>
+  </si>
+  <si>
+    <t>no internal error / no error of any Test Trigger</t>
+  </si>
+  <si>
+    <t>-x (with x is the number of  failed Test Trigger selftest usecases)</t>
+  </si>
+  <si>
+    <t>continue with next Test Trigger selftest usecases
+(until last usecase reached)</t>
+  </si>
+  <si>
     <t>continue with next Executor
-(until last reached)</t>
-  </si>
-  <si>
-    <t>-x (with x is the number of  Executors who returned a value != 0)</t>
+(until last Executor reached)</t>
   </si>
 </sst>
 </file>
@@ -129,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -259,9 +282,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -301,6 +321,33 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -326,13 +373,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>6349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -347,8 +394,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="863600" y="190500"/>
-          <a:ext cx="7969250" cy="4127500"/>
+          <a:off x="863600" y="196849"/>
+          <a:ext cx="7969250" cy="4918075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -393,7 +440,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-DE" sz="1100"/>
-            <a:t>V 0.2.0 / 30.09.2022</a:t>
+            <a:t>V 0.3.0 / 21.10.2022</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -780,6 +827,77 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>Database Executor writes to the database.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>→ Test Trigger self test calls</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> the Test Trigger with several combinations of several command lines and configurations.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1382,9 +1500,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92586ADF-3908-4DA7-9882-F5B92A2A2740}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1396,19 +1516,19 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1422,194 +1542,221 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="10"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="22">
         <v>0</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="8"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>0</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="18"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>0</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
-      <c r="B16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="14">
+      <c r="B18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="27">
         <v>0</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D20" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="10"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>